<commit_message>
Re-run of output tables
</commit_message>
<xml_diff>
--- a/final-outputs/Table B Individual.xlsx
+++ b/final-outputs/Table B Individual.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="223">
   <si>
     <t>country</t>
   </si>
@@ -296,7 +296,7 @@
     <t>55.0%</t>
   </si>
   <si>
-    <t>52.9%</t>
+    <t>60.2%</t>
   </si>
   <si>
     <t>53.5%</t>
@@ -305,289 +305,307 @@
     <t>35.0%</t>
   </si>
   <si>
+    <t>31.1%</t>
+  </si>
+  <si>
+    <t>55.9%</t>
+  </si>
+  <si>
+    <t>32.4%</t>
+  </si>
+  <si>
+    <t>58.4%</t>
+  </si>
+  <si>
+    <t>55.6%</t>
+  </si>
+  <si>
+    <t>47.5%</t>
+  </si>
+  <si>
+    <t>33.5%</t>
+  </si>
+  <si>
+    <t>44.4%</t>
+  </si>
+  <si>
+    <t>52.0%</t>
+  </si>
+  <si>
+    <t>50.0%</t>
+  </si>
+  <si>
+    <t>52.8%</t>
+  </si>
+  <si>
+    <t>56.1%</t>
+  </si>
+  <si>
+    <t>47.4%</t>
+  </si>
+  <si>
+    <t>38.9%</t>
+  </si>
+  <si>
+    <t>24.0%</t>
+  </si>
+  <si>
+    <t>47.2%</t>
+  </si>
+  <si>
+    <t>52.3%</t>
+  </si>
+  <si>
+    <t>33.0%</t>
+  </si>
+  <si>
+    <t>46.6%</t>
+  </si>
+  <si>
+    <t>39.9%</t>
+  </si>
+  <si>
+    <t>58.2%</t>
+  </si>
+  <si>
+    <t>61.1%</t>
+  </si>
+  <si>
+    <t>43.5%</t>
+  </si>
+  <si>
+    <t>60.1%</t>
+  </si>
+  <si>
+    <t>41.7%</t>
+  </si>
+  <si>
+    <t>45.5%</t>
+  </si>
+  <si>
+    <t>46.0%</t>
+  </si>
+  <si>
+    <t>Top Income Tax Rate Threshold (a)</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>23.3</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>14.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>28.7</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>15.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Ratio of Marginal to Average Tax Wedge</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Income Tax Complexity</t>
+  </si>
+  <si>
+    <t>Income Tax Complexity (Payments)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Income Tax Complexity (Time)</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Capital Gains/Dividends</t>
+  </si>
+  <si>
+    <t>Top Marginal Capital Gains Rate (b)</t>
+  </si>
+  <si>
+    <t>24.5%</t>
+  </si>
+  <si>
+    <t>27.5%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>26.8%</t>
+  </si>
+  <si>
     <t>15.0%</t>
   </si>
   <si>
-    <t>55.9%</t>
+    <t>42.0%</t>
   </si>
   <si>
     <t>20.0%</t>
   </si>
   <si>
-    <t>51.1%</t>
-  </si>
-  <si>
-    <t>55.4%</t>
-  </si>
-  <si>
-    <t>47.5%</t>
-  </si>
-  <si>
-    <t>46.2%</t>
-  </si>
-  <si>
-    <t>48.0%</t>
-  </si>
-  <si>
-    <t>50.0%</t>
-  </si>
-  <si>
-    <t>47.2%</t>
-  </si>
-  <si>
-    <t>31.4%</t>
-  </si>
-  <si>
-    <t>45.8%</t>
-  </si>
-  <si>
-    <t>51.9%</t>
-  </si>
-  <si>
-    <t>33.0%</t>
-  </si>
-  <si>
-    <t>38.4%</t>
-  </si>
-  <si>
-    <t>32.0%</t>
-  </si>
-  <si>
-    <t>53.0%</t>
+    <t>34.0%</t>
+  </si>
+  <si>
+    <t>30.0%</t>
+  </si>
+  <si>
+    <t>26.4%</t>
   </si>
   <si>
     <t>25.0%</t>
-  </si>
-  <si>
-    <t>43.5%</t>
-  </si>
-  <si>
-    <t>57.1%</t>
-  </si>
-  <si>
-    <t>41.7%</t>
-  </si>
-  <si>
-    <t>35.8%</t>
-  </si>
-  <si>
-    <t>45.0%</t>
-  </si>
-  <si>
-    <t>43.6%</t>
-  </si>
-  <si>
-    <t>Top Income Tax Rate Threshold (a)</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>23.3</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>14.3</t>
-  </si>
-  <si>
-    <t>5.4</t>
-  </si>
-  <si>
-    <t>11.0</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>2.7</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>11.4</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>28.7</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>15.3</t>
-  </si>
-  <si>
-    <t>3.4</t>
-  </si>
-  <si>
-    <t>4.8</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
-    <t>9.3</t>
-  </si>
-  <si>
-    <t>Ratio of Marginal to Average Tax Wedge</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>Income Tax Complexity</t>
-  </si>
-  <si>
-    <t>Income Tax Complexity (Payments)</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Income Tax Complexity (Time)</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>169</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>Capital Gains/Dividends</t>
-  </si>
-  <si>
-    <t>Top Marginal Capital Gains Rate (b)</t>
-  </si>
-  <si>
-    <t>24.5%</t>
-  </si>
-  <si>
-    <t>27.5%</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>26.8%</t>
-  </si>
-  <si>
-    <t>42.0%</t>
-  </si>
-  <si>
-    <t>34.0%</t>
-  </si>
-  <si>
-    <t>30.0%</t>
-  </si>
-  <si>
-    <t>26.4%</t>
   </si>
   <si>
     <t>22.0%</t>
@@ -757,13 +775,13 @@
         <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I2" t="s">
         <v>49</v>
@@ -780,22 +798,22 @@
         <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="I3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
@@ -809,10 +827,10 @@
         <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -821,10 +839,10 @@
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5">
@@ -838,22 +856,22 @@
         <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6">
@@ -867,10 +885,10 @@
         <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -879,10 +897,10 @@
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7">
@@ -896,10 +914,10 @@
         <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -908,10 +926,10 @@
         <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I7" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8">
@@ -925,22 +943,22 @@
         <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H8" t="s">
         <v>96</v>
       </c>
       <c r="I8" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9">
@@ -954,22 +972,22 @@
         <v>97</v>
       </c>
       <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" t="s">
         <v>127</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="I9" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10">
@@ -983,22 +1001,22 @@
         <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11">
@@ -1012,22 +1030,22 @@
         <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G11" t="s">
         <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="I11" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12">
@@ -1041,22 +1059,22 @@
         <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E12" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="I12" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13">
@@ -1070,22 +1088,22 @@
         <v>101</v>
       </c>
       <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
         <v>131</v>
-      </c>
-      <c r="E13" t="s">
-        <v>128</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="I13" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14">
@@ -1099,22 +1117,22 @@
         <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="I14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15">
@@ -1128,22 +1146,22 @@
         <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16">
@@ -1154,25 +1172,25 @@
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="I16" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17">
@@ -1183,25 +1201,25 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="I17" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18">
@@ -1212,13 +1230,13 @@
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -1227,10 +1245,10 @@
         <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19">
@@ -1241,25 +1259,25 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E19" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H19" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="I19" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20">
@@ -1270,25 +1288,25 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
         <v>138</v>
-      </c>
-      <c r="E20" t="s">
-        <v>135</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21">
@@ -1299,25 +1317,25 @@
         <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="I21" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22">
@@ -1328,25 +1346,25 @@
         <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H22" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I22" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23">
@@ -1357,25 +1375,25 @@
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="I23" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24">
@@ -1386,13 +1404,13 @@
         <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -1401,10 +1419,10 @@
         <v>41</v>
       </c>
       <c r="H24" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="I24" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25">
@@ -1415,13 +1433,13 @@
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1430,10 +1448,10 @@
         <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I25" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26">
@@ -1447,10 +1465,10 @@
         <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1459,10 +1477,10 @@
         <v>45</v>
       </c>
       <c r="H26" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="I26" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27">
@@ -1473,25 +1491,25 @@
         <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H27" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28">
@@ -1502,25 +1520,25 @@
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H28" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I28" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29">
@@ -1531,13 +1549,13 @@
         <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1546,10 +1564,10 @@
         <v>22</v>
       </c>
       <c r="H29" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I29" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30">
@@ -1560,25 +1578,25 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H30" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="I30" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31">
@@ -1589,25 +1607,25 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H31" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="I31" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32">
@@ -1618,25 +1636,25 @@
         <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H32" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I32" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33">
@@ -1647,25 +1665,25 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H33" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I33" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34">
@@ -1676,25 +1694,25 @@
         <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H34" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="I34" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35">
@@ -1705,13 +1723,13 @@
         <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
@@ -1720,10 +1738,10 @@
         <v>43</v>
       </c>
       <c r="H35" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="I35" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36">
@@ -1734,13 +1752,13 @@
         <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -1749,10 +1767,10 @@
         <v>47</v>
       </c>
       <c r="H36" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I36" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37">
@@ -1763,25 +1781,25 @@
         <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H37" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38">
@@ -1792,25 +1810,25 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H38" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="I38" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39">
@@ -1821,25 +1839,25 @@
         <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H39" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40">

</xml_diff>